<commit_message>
PE 3.8 ACUITY TASK AND EVENT
Signed-off-by: sahilbansal <sbansal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/API Files/Acuity(call task and event)/Account.xlsx
+++ b/API Files/Acuity(call task and event)/Account.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil Bansal\git\PE4.7Automation\API Files\Acuity(call task and event)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil Bansal.DESK0090\git\PE4.7Automation\API Files\Acuity(call task and event)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42CCFE3F-033F-45C9-83F2-D3DB106E1C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView windowHeight="12450" windowWidth="23250" xWindow="-105" yWindow="-105"/>
   </bookViews>
   <sheets>
-    <sheet name="Account Success" sheetId="1" r:id="rId1"/>
+    <sheet name="Account" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Test Account 1_COMPANY</t>
   </si>
@@ -100,14 +99,15 @@
     <t>navpeII__Entity_Type__c</t>
   </si>
   <si>
-    <t>navpeII__Tier__c</t>
+    <t>Created</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +241,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -541,98 +547,99 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="5" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="6" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="7" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="8" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="19"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="23"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="27"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="31"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="35"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="39"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="20"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="24"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="28"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="32"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="36"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="40"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="21"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="25"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="29"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="33"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="37"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="41"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="18"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="22"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="26"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="30"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="34"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="38"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="7"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="11"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="13"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="16"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="6"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="2"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="3"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="4"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="5"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="9"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="12"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="15"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="10"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="1"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="17"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -649,10 +656,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -687,7 +694,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -739,7 +746,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -850,21 +857,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -881,7 +888,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -933,23 +940,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -962,25 +969,25 @@
       <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -990,11 +997,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1004,11 +1011,11 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1018,11 +1025,11 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1032,11 +1039,11 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1046,11 +1053,11 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1068,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -1072,7 +1082,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -1082,11 +1095,11 @@
       <c r="D10" t="s">
         <v>2</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -1096,11 +1109,11 @@
       <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1110,11 +1123,11 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -1124,11 +1137,11 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -1138,11 +1151,11 @@
       <c r="D14" t="s">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1152,12 +1165,9 @@
       <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>